<commit_message>
fix formula cell cannot convert to object
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsx/test.xlsx
+++ b/src/test/resources/xlsx/test.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>number</t>
   </si>
@@ -23,6 +23,15 @@
   </si>
   <si>
     <t>날짜</t>
+  </si>
+  <si>
+    <t>formula</t>
+  </si>
+  <si>
+    <t>formula2</t>
+  </si>
+  <si>
+    <t>date_time</t>
   </si>
   <si>
     <t>이순신</t>
@@ -41,8 +50,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy. M. d"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="yyyy. mm. dd h:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="yyyy. m. d h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -71,7 +83,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -79,6 +91,16 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -296,6 +318,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="6" max="7" width="17.25"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -310,6 +335,15 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1">
@@ -319,10 +353,21 @@
         <v>11.0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2">
         <v>44853.0</v>
+      </c>
+      <c r="E2" s="3">
+        <f t="shared" ref="E2:E5" si="1">A2+B2</f>
+        <v>12</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f t="shared" ref="F2:F5" si="2">E2/(A2-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G2" s="5">
+        <v>44197.54194444444</v>
       </c>
     </row>
     <row r="3">
@@ -333,10 +378,21 @@
         <v>12.0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2">
         <v>44854.0</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="G3" s="5">
+        <v>30371.041944444445</v>
       </c>
     </row>
     <row r="4">
@@ -347,10 +403,21 @@
         <v>13.0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2">
         <v>44855.0</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G4" s="6">
+        <v>44217.0</v>
       </c>
     </row>
     <row r="5">
@@ -361,10 +428,21 @@
         <v>14.0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
         <v>44856.0</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G5" s="5">
+        <v>44200.54194444444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix multi-line header table to object
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsx/test.xlsx
+++ b/src/test/resources/xlsx/test.xlsx
@@ -4,6 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="시트1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="2line_header_1line_content" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="2line_header_2line_content" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="2line_header_2line_content_2" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t>number</t>
   </si>
@@ -44,6 +47,30 @@
   </si>
   <si>
     <t>특_수_문_자</t>
+  </si>
+  <si>
+    <t>숫자</t>
+  </si>
+  <si>
+    <t>공식</t>
+  </si>
+  <si>
+    <t>시간</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>일시</t>
+  </si>
+  <si>
+    <t>별명</t>
+  </si>
+  <si>
+    <t>미스터리</t>
+  </si>
+  <si>
+    <t>제임스</t>
   </si>
 </sst>
 </file>
@@ -56,7 +83,7 @@
     <numFmt numFmtId="166" formatCode="yyyy. mm. dd h:mm:ss"/>
     <numFmt numFmtId="167" formatCode="yyyy. m. d h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -67,6 +94,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -102,6 +133,33 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -112,6 +170,18 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -448,4 +518,589 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" ref="E5:E8" si="1">B5+C5</f>
+        <v>12</v>
+      </c>
+      <c r="F5" s="9" t="str">
+        <f t="shared" ref="F5:F8" si="2">E5/(B5-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="10">
+        <v>44853.0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>44197.54194444444</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="G6" s="10">
+        <v>44854.0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>30371.041944444445</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G7" s="10">
+        <v>44855.0</v>
+      </c>
+      <c r="H7" s="13">
+        <v>44217.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G8" s="10">
+        <v>44856.0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>44200.54194444444</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7"/>
+      <c r="B5" s="15">
+        <v>-1.0</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="8" t="str">
+        <f>sum(E6, F6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="10">
+        <f>min(G6, H6)</f>
+        <v>44197.54194</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="8">
+        <f>B6+C6</f>
+        <v>12</v>
+      </c>
+      <c r="F6" s="9" t="str">
+        <f>E6/(B6-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" s="10">
+        <v>44853.0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>44197.54194444444</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7"/>
+      <c r="B7" s="15">
+        <v>-2.0</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="8">
+        <f>sum(E8, F8)</f>
+        <v>28</v>
+      </c>
+      <c r="G7" s="10">
+        <f>min(G8, H8)</f>
+        <v>30371.04194</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="8">
+        <f>B8+C8</f>
+        <v>14</v>
+      </c>
+      <c r="F8" s="12">
+        <f>E8/(B8-1)</f>
+        <v>14</v>
+      </c>
+      <c r="G8" s="10">
+        <v>44854.0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>30371.041944444445</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="7"/>
+      <c r="B7" s="15">
+        <v>-1.0</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8" t="str">
+        <f>sum(E8, F8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" s="10">
+        <f>min(G8, H8)</f>
+        <v>44197.54194</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="8">
+        <f>B8+C8</f>
+        <v>12</v>
+      </c>
+      <c r="F8" s="9" t="str">
+        <f>E8/(B8-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="10">
+        <v>44853.0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>44197.54194444444</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7"/>
+      <c r="B9" s="15">
+        <v>-2.0</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="8">
+        <f>sum(E10, F10)</f>
+        <v>28</v>
+      </c>
+      <c r="G9" s="10">
+        <f>min(G10, H10)</f>
+        <v>30371.04194</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="8">
+        <f>B10+C10</f>
+        <v>14</v>
+      </c>
+      <c r="F10" s="12">
+        <f>E10/(B10-1)</f>
+        <v>14</v>
+      </c>
+      <c r="G10" s="10">
+        <v>44854.0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>30371.041944444445</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix multi-line header table to object (#2)
* fix multi-line header table to object

* fix multi-line header table to object by setter
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsx/test.xlsx
+++ b/src/test/resources/xlsx/test.xlsx
@@ -4,6 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="시트1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="2line_header_1line_content" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="2line_header_2line_content" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="2line_header_2line_content_2" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
   <si>
     <t>number</t>
   </si>
@@ -44,6 +47,30 @@
   </si>
   <si>
     <t>특_수_문_자</t>
+  </si>
+  <si>
+    <t>숫자</t>
+  </si>
+  <si>
+    <t>공식</t>
+  </si>
+  <si>
+    <t>시간</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>일시</t>
+  </si>
+  <si>
+    <t>별명</t>
+  </si>
+  <si>
+    <t>미스터리</t>
+  </si>
+  <si>
+    <t>제임스</t>
   </si>
 </sst>
 </file>
@@ -56,7 +83,7 @@
     <numFmt numFmtId="166" formatCode="yyyy. mm. dd h:mm:ss"/>
     <numFmt numFmtId="167" formatCode="yyyy. m. d h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -67,6 +94,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -102,6 +133,33 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="167" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -112,6 +170,18 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -448,4 +518,589 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" ref="E5:E8" si="1">B5+C5</f>
+        <v>12</v>
+      </c>
+      <c r="F5" s="9" t="str">
+        <f t="shared" ref="F5:F8" si="2">E5/(B5-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="10">
+        <v>44853.0</v>
+      </c>
+      <c r="H5" s="11">
+        <v>44197.54194444444</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="F6" s="12">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="G6" s="10">
+        <v>44854.0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>30371.041944444445</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F7" s="12">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="G7" s="10">
+        <v>44855.0</v>
+      </c>
+      <c r="H7" s="13">
+        <v>44217.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="G8" s="10">
+        <v>44856.0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>44200.54194444444</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7"/>
+      <c r="B5" s="15">
+        <v>-1.0</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="8" t="str">
+        <f>sum(E6, F6)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="10">
+        <f>min(G6, H6)</f>
+        <v>44197.54194</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="8">
+        <f>B6+C6</f>
+        <v>12</v>
+      </c>
+      <c r="F6" s="9" t="str">
+        <f>E6/(B6-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G6" s="10">
+        <v>44853.0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>44197.54194444444</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="7"/>
+      <c r="B7" s="15">
+        <v>-2.0</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="8">
+        <f>sum(E8, F8)</f>
+        <v>28</v>
+      </c>
+      <c r="G7" s="10">
+        <f>min(G8, H8)</f>
+        <v>30371.04194</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="8">
+        <f>B8+C8</f>
+        <v>14</v>
+      </c>
+      <c r="F8" s="12">
+        <f>E8/(B8-1)</f>
+        <v>14</v>
+      </c>
+      <c r="G8" s="10">
+        <v>44854.0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>30371.041944444445</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="7"/>
+      <c r="B7" s="15">
+        <v>-1.0</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="8" t="str">
+        <f>sum(E8, F8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" s="10">
+        <f>min(G8, H8)</f>
+        <v>44197.54194</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="8">
+        <f>B8+C8</f>
+        <v>12</v>
+      </c>
+      <c r="F8" s="9" t="str">
+        <f>E8/(B8-1)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="10">
+        <v>44853.0</v>
+      </c>
+      <c r="H8" s="11">
+        <v>44197.54194444444</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="7"/>
+      <c r="B9" s="15">
+        <v>-2.0</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="8">
+        <f>sum(E10, F10)</f>
+        <v>28</v>
+      </c>
+      <c r="G9" s="10">
+        <f>min(G10, H10)</f>
+        <v>30371.04194</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="C10" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="8">
+        <f>B10+C10</f>
+        <v>14</v>
+      </c>
+      <c r="F10" s="12">
+        <f>E10/(B10-1)</f>
+        <v>14</v>
+      </c>
+      <c r="G10" s="10">
+        <v>44854.0</v>
+      </c>
+      <c r="H10" s="11">
+        <v>30371.041944444445</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+  </mergeCells>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>